<commit_message>
correct turn comments and add cruise speed line from exel to MATLAB
</commit_message>
<xml_diff>
--- a/figure/Cruise Speed line.xlsx
+++ b/figure/Cruise Speed line.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\University\karshenasi\Aircraft Design\Project\Phase#2\Report\Projects Pack v2-1 Date 13970820\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\figure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC93E87-8C13-4988-8588-678BF4C0CDD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672874F-822B-4786-8DCB-58EC22AB5161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Medium" sheetId="1" r:id="rId1"/>
@@ -7038,13 +7038,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7058,7 +7058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
@@ -7082,7 +7082,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>2.5885166925684749E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>2.4522800531771565E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>2.3473996287579148E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>2.2666393697018086E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>2.2048306691453093E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
@@ -7402,7 +7402,7 @@
         <v>2.1581832153884956E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>2.1238542746564264E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>2.0996699917094405E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>2.0839395902500241E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>2.075328246885404E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>2.0727681029013595E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>2.0753947012435235E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>2.0825007588674123E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>2.0935019984754107E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>2.1079115223195038E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>2.1253203362913611E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>2.145382368453163E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>2.1678028167838051E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>2.1923289938366255E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>2.2187430656058819E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
@@ -7660,9 +7660,9 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7676,7 +7676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
@@ -7700,7 +7700,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
@@ -7868,7 +7868,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>2.6178944192332722E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
@@ -7956,7 +7956,7 @@
         <v>2.4845955525084333E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>2.3826529007556711E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>2.3048304143660447E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>2.2459594864760252E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>2.202249805385691E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>2.1708586373201017E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>2.1496121270395956E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>2.1368194982466591E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>2.1311459275485185E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>2.1315235562309534E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>2.1370879272395969E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>2.1471317575299662E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>2.1610707698044438E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>2.1784180663150167E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>2.1987646529533538E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>2.2217644577816352E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>2.2471226787787572E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>2.2745866284980574E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
@@ -8244,7 +8244,7 @@
         <v>2.3039384729337933E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
@@ -8274,13 +8274,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
@@ -8318,7 +8318,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
@@ -8458,7 +8458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
@@ -8542,7 +8542,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
@@ -8558,7 +8558,7 @@
         <v>2.5621265313272166E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>2.4232508758117725E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>2.3157314352684043E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>2.2323321600881726E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>2.1678844434075476E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>2.1185979735266078E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>2.0816300166704129E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>2.0548067175993015E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>2.0364373000157594E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>2.0251869405270129E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>2.0199877804188429E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>2.0199753626368808E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>2.0244424041366442E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>2.0328046276205162E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>2.0445751353404835E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>2.0593449331882147E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>2.0767679492258911E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>2.0965493814324072E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>2.1184365423611021E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>2.1422115980062328E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
@@ -8878,10 +8878,10 @@
         <v>2.1676857588961557E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add max Cruise speed line fix loverd max
</commit_message>
<xml_diff>
--- a/figure/Cruise Speed line.xlsx
+++ b/figure/Cruise Speed line.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Airplane-Design-II\figure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672874F-822B-4786-8DCB-58EC22AB5161}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Medium" sheetId="1" r:id="rId1"/>
     <sheet name="Low" sheetId="2" r:id="rId2"/>
     <sheet name="High" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,12 +67,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -82,7 +81,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -90,7 +89,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -98,7 +97,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -106,7 +105,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -115,7 +114,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -273,6 +272,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -298,7 +298,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -441,94 +441,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20589030128179339</c:v>
+                  <c:v>0.19974070727068258</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10380782222850723</c:v>
+                  <c:v>0.10073302522295183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0163738805238768E-2</c:v>
+                  <c:v>6.8113874134868496E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3629254289474716E-2</c:v>
+                  <c:v>5.2091855786697012E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3938609336712432E-2</c:v>
+                  <c:v>4.2708690534490265E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7669884165451029E-2</c:v>
+                  <c:v>3.6644951830265886E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3356541726475848E-2</c:v>
+                  <c:v>3.2478028296317157E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0265313495179549E-2</c:v>
+                  <c:v>2.9496614243790697E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7988828069002509E-2</c:v>
+                  <c:v>2.7305539845545752E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6282662606408956E-2</c:v>
+                  <c:v>2.5667703205297872E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4991275299148834E-2</c:v>
+                  <c:v>2.4432221298138764E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.4010971608388797E-2</c:v>
+                  <c:v>2.3498505440796229E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.326996300724421E-2</c:v>
+                  <c:v>2.2796917314081837E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2716971976511756E-2</c:v>
+                  <c:v>2.227771526143241E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2314395002109008E-2</c:v>
+                  <c:v>2.1904422068034956E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.203402944847415E-2</c:v>
+                  <c:v>2.1649679822779728E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1854308594295206E-2</c:v>
+                  <c:v>2.1492567770112218E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1758458322996183E-2</c:v>
+                  <c:v>2.1416814211267805E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1733235910964464E-2</c:v>
+                  <c:v>2.1409573068274422E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1768047179309954E-2</c:v>
+                  <c:v>2.1460567478754411E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1854315887978759E-2</c:v>
+                  <c:v>2.1561478077925866E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1985025113290438E-2</c:v>
+                  <c:v>2.1705498112785406E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2154378266117655E-2</c:v>
+                  <c:v>2.1887004613460666E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.235754485552097E-2</c:v>
+                  <c:v>2.2101311771724683E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2590467269111247E-2</c:v>
+                  <c:v>2.2344483508666815E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2849712142559223E-2</c:v>
+                  <c:v>2.2613189295978036E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3132354758102928E-2</c:v>
+                  <c:v>2.2904592016950678E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3435888214803545E-2</c:v>
+                  <c:v>2.3216259857263874E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3758151391162066E-2</c:v>
+                  <c:v>2.3546096425261693E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4097271315212717E-2</c:v>
+                  <c:v>2.3892284848175689E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,7 +606,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="640747376"/>
@@ -682,7 +682,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="640751968"/>
@@ -723,7 +723,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -777,6 +777,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -802,7 +803,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -945,94 +946,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20747002532011743</c:v>
+                  <c:v>0.21762362435295637</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10451352241667586</c:v>
+                  <c:v>0.10959032193309533</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0540692451802917E-2</c:v>
+                  <c:v>7.3925225462749253E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3813780721572162E-2</c:v>
+                  <c:v>5.6352180479781896E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3985236285198279E-2</c:v>
+                  <c:v>4.6015956091766078E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7605875495752825E-2</c:v>
+                  <c:v>3.9298142001225986E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3197476790266481E-2</c:v>
+                  <c:v>3.4647990937814906E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0020929387254574E-2</c:v>
+                  <c:v>3.1290129266359441E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7665616185892292E-2</c:v>
+                  <c:v>2.8793793856207731E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5885166925684749E-2</c:v>
+                  <c:v>2.6900526828968648E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4522800531771565E-2</c:v>
+                  <c:v>2.544585498930238E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3473996287579148E-2</c:v>
+                  <c:v>2.4320129540315726E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2666393697018086E-2</c:v>
+                  <c:v>2.3447439776467238E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2048306691453093E-2</c:v>
+                  <c:v>2.2773563765227305E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1581832153884956E-2</c:v>
+                  <c:v>2.2258738756074221E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1238542746564264E-2</c:v>
+                  <c:v>2.1873142686116696E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0996699917094405E-2</c:v>
+                  <c:v>2.1593970448437871E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0839395902500241E-2</c:v>
+                  <c:v>2.1403484737657963E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.075328246885404E-2</c:v>
+                  <c:v>2.1287682417950829E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0727681029013595E-2</c:v>
+                  <c:v>2.1235360980655545E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0753947012435235E-2</c:v>
+                  <c:v>2.1237451728284708E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0825007588674123E-2</c:v>
+                  <c:v>2.1286534817439532E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0935019984754107E-2</c:v>
+                  <c:v>2.1376480812268846E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1079115223195038E-2</c:v>
+                  <c:v>2.1502181849563328E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.1253203362913611E-2</c:v>
+                  <c:v>2.1659347324227165E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.145382368453163E-2</c:v>
+                  <c:v>2.1844346724256204E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.1678028167838051E-2</c:v>
+                  <c:v>2.2054087391276532E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.1923289938366255E-2</c:v>
+                  <c:v>2.2285918475253363E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2187430656058819E-2</c:v>
+                  <c:v>2.2537554760639473E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2468562426199309E-2</c:v>
+                  <c:v>2.280701572729394E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1110,7 +1111,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="540720312"/>
@@ -1186,7 +1187,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="540719984"/>
@@ -1227,7 +1228,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1283,6 +1284,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1308,7 +1310,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1451,94 +1453,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20592285492660886</c:v>
+                  <c:v>0.19977326091549807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10387292951813822</c:v>
+                  <c:v>0.10079813251258282</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0261399739685246E-2</c:v>
+                  <c:v>6.8211535069314974E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3759468868736678E-2</c:v>
+                  <c:v>5.2222070365958981E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4101377560789898E-2</c:v>
+                  <c:v>4.2871458758567731E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7865206034343978E-2</c:v>
+                  <c:v>3.6840273699158842E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3584417240184287E-2</c:v>
+                  <c:v>3.2705903810025604E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0525742653703485E-2</c:v>
+                  <c:v>2.9757043402314633E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8281810872341943E-2</c:v>
+                  <c:v>2.7598522648885185E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.660819905456388E-2</c:v>
+                  <c:v>2.5993239653452797E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5349365392119252E-2</c:v>
+                  <c:v>2.4790311391109179E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.4401615346174708E-2</c:v>
+                  <c:v>2.3889149178582141E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3693160389845608E-2</c:v>
+                  <c:v>2.3220114696683242E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3172723003928648E-2</c:v>
+                  <c:v>2.2733466288849306E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2802699674341394E-2</c:v>
+                  <c:v>2.2392726740267339E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.255488776552203E-2</c:v>
+                  <c:v>2.2170538139827604E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2407720556158577E-2</c:v>
+                  <c:v>2.2045979731975588E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2344423929675044E-2</c:v>
+                  <c:v>2.2002779817946669E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2351755162458822E-2</c:v>
+                  <c:v>2.2028092319768777E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2419120075619799E-2</c:v>
+                  <c:v>2.2111640375064259E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2537942429104101E-2</c:v>
+                  <c:v>2.2245104619051208E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.270120529923127E-2</c:v>
+                  <c:v>2.2421678298726239E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2903112096873981E-2</c:v>
+                  <c:v>2.2635738444216989E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3138832331092787E-2</c:v>
+                  <c:v>2.2882599247296503E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3404308389498554E-2</c:v>
+                  <c:v>2.3158324629054126E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3696106907762023E-2</c:v>
+                  <c:v>2.3459584061180837E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4011303168121223E-2</c:v>
+                  <c:v>2.3783540426968973E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.434739026963733E-2</c:v>
+                  <c:v>2.4127761912097659E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4702207090811348E-2</c:v>
+                  <c:v>2.4490152124910975E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5073880659677493E-2</c:v>
+                  <c:v>2.4868894192640465E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1616,7 +1618,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="523088608"/>
@@ -1678,7 +1680,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="523081392"/>
@@ -1719,7 +1721,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1775,6 +1777,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1800,7 +1803,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1943,94 +1946,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20749940304678224</c:v>
+                  <c:v>0.21765300207962118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10457227787000545</c:v>
+                  <c:v>0.10964907738642492</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0628825631797315E-2</c:v>
+                  <c:v>7.4013358642743637E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3931291628231362E-2</c:v>
+                  <c:v>5.6469691386441097E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4132124918522267E-2</c:v>
+                  <c:v>4.6162844725090066E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7782141855741608E-2</c:v>
+                  <c:v>3.9474408361214776E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3403120876920059E-2</c:v>
+                  <c:v>3.4853635024468484E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0255951200572947E-2</c:v>
+                  <c:v>3.1525151079677814E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7930015725875463E-2</c:v>
+                  <c:v>2.9058193396190906E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6178944192332722E-2</c:v>
+                  <c:v>2.7194304095616621E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4845955525084333E-2</c:v>
+                  <c:v>2.5769009982615151E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3826529007556711E-2</c:v>
+                  <c:v>2.4672662260293292E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3048304143660447E-2</c:v>
+                  <c:v>2.3829350223109599E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2459594864760252E-2</c:v>
+                  <c:v>2.3184851938534465E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.202249805385691E-2</c:v>
+                  <c:v>2.2699404656046175E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1708586373201017E-2</c:v>
+                  <c:v>2.2343186312753449E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1496121270395956E-2</c:v>
+                  <c:v>2.2093391801739422E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1368194982466591E-2</c:v>
+                  <c:v>2.1932283817624312E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1311459275485185E-2</c:v>
+                  <c:v>2.184585922458197E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1315235562309534E-2</c:v>
+                  <c:v>2.1822915513951484E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1370879272395969E-2</c:v>
+                  <c:v>2.1854383988245449E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1471317575299662E-2</c:v>
+                  <c:v>2.1932844804065068E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1610707698044438E-2</c:v>
+                  <c:v>2.2052168525559173E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1784180663150167E-2</c:v>
+                  <c:v>2.2207247289518457E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.1987646529533538E-2</c:v>
+                  <c:v>2.2393790490847092E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2217644577816352E-2</c:v>
+                  <c:v>2.260816761754093E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2471226787787572E-2</c:v>
+                  <c:v>2.2847286011226053E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2745866284980574E-2</c:v>
+                  <c:v>2.3108494821867675E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3039384729337933E-2</c:v>
+                  <c:v>2.338950883391859E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3349894226143222E-2</c:v>
+                  <c:v>2.3688347527237853E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2108,7 +2111,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="616388416"/>
@@ -2170,7 +2173,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="616386120"/>
@@ -2211,7 +2214,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2267,6 +2270,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2292,7 +2296,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2435,94 +2439,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20586105817712863</c:v>
+                  <c:v>0.19971146416601782</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1037493360191777</c:v>
+                  <c:v>0.10067453901362231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0076009491244484E-2</c:v>
+                  <c:v>6.8026144820874213E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3512281870815658E-2</c:v>
+                  <c:v>5.1974883368037961E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3792393813388612E-2</c:v>
+                  <c:v>4.2562475011166452E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7494425537462441E-2</c:v>
+                  <c:v>3.6469493202277305E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3151839993822492E-2</c:v>
+                  <c:v>3.2273326563663808E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0031368657861435E-2</c:v>
+                  <c:v>2.9262669406472583E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.772564012701963E-2</c:v>
+                  <c:v>2.7042351903562876E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5990231559761313E-2</c:v>
+                  <c:v>2.5375272158650229E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4669601147836426E-2</c:v>
+                  <c:v>2.4110547146826353E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3660054352411627E-2</c:v>
+                  <c:v>2.314758818481906E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2889802646602272E-2</c:v>
+                  <c:v>2.2416756953439903E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2307568511205054E-2</c:v>
+                  <c:v>2.1868311796125712E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1875748432137545E-2</c:v>
+                  <c:v>2.1465775498063493E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1566139773837922E-2</c:v>
+                  <c:v>2.11817901481435E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1357175814994214E-2</c:v>
+                  <c:v>2.0995434990811222E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1232082439030426E-2</c:v>
+                  <c:v>2.0890438327302047E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1177616922333942E-2</c:v>
+                  <c:v>2.08539540796439E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1183185086014664E-2</c:v>
+                  <c:v>2.0875705385459124E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1240210690018708E-2</c:v>
+                  <c:v>2.0947372879965814E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1341676810665625E-2</c:v>
+                  <c:v>2.1062149810160587E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1481786858828077E-2</c:v>
+                  <c:v>2.1214413206171085E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1655710343566628E-2</c:v>
+                  <c:v>2.1399477259770341E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.185938965249214E-2</c:v>
+                  <c:v>2.1613405892047705E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2089391421275351E-2</c:v>
+                  <c:v>2.1852868574694165E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2342790932154293E-2</c:v>
+                  <c:v>2.2115028191002042E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2617081284190141E-2</c:v>
+                  <c:v>2.239745292665047E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2910101355883904E-2</c:v>
+                  <c:v>2.2698046389983535E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3219978175269787E-2</c:v>
+                  <c:v>2.3014991708232759E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2600,7 +2604,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="627630560"/>
@@ -2662,7 +2666,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="627628592"/>
@@ -2703,7 +2707,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2759,6 +2763,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2784,7 +2789,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fa-IR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2927,94 +2932,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.20744363515887621</c:v>
+                  <c:v>0.21759723419171514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10446074209419333</c:v>
+                  <c:v>0.1095375416106128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0461521968079144E-2</c:v>
+                  <c:v>7.384605497902548E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3708220076607131E-2</c:v>
+                  <c:v>5.6246619834816873E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3853285478991991E-2</c:v>
+                  <c:v>4.588400528555979E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7447534528305272E-2</c:v>
+                  <c:v>3.913980103377844E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3012745661577671E-2</c:v>
+                  <c:v>3.4463259809126096E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9809808097324503E-2</c:v>
+                  <c:v>3.107900797642937E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7428104734720966E-2</c:v>
+                  <c:v>2.8556282405036409E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5621265313272166E-2</c:v>
+                  <c:v>2.6636625216556065E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4232508758117725E-2</c:v>
+                  <c:v>2.515556321564854E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3157314352684043E-2</c:v>
+                  <c:v>2.4003447605420627E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2323321600881726E-2</c:v>
+                  <c:v>2.3104367680330879E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1678844434075476E-2</c:v>
+                  <c:v>2.2404101507849689E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1185979735266078E-2</c:v>
+                  <c:v>2.1862886337455343E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0816300166704129E-2</c:v>
+                  <c:v>2.1450900106256564E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.0548067175993015E-2</c:v>
+                  <c:v>2.1145337707336478E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.0364373000157594E-2</c:v>
+                  <c:v>2.0928461835315316E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0251869405270129E-2</c:v>
+                  <c:v>2.0786269354366917E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0199877804188429E-2</c:v>
+                  <c:v>2.0707557755830379E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0199753626368808E-2</c:v>
+                  <c:v>2.0683258342218284E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0244424041366442E-2</c:v>
+                  <c:v>2.0705951270131851E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0328046276205162E-2</c:v>
+                  <c:v>2.07695071037199E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.0445751353404835E-2</c:v>
+                  <c:v>2.0868817979773125E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.0593449331882147E-2</c:v>
+                  <c:v>2.0999593293195708E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.0767679492258911E-2</c:v>
+                  <c:v>2.1158202531983489E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.0965493814324072E-2</c:v>
+                  <c:v>2.1341553037762556E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.1184365423611021E-2</c:v>
+                  <c:v>2.1546993960498126E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.1422115980062328E-2</c:v>
+                  <c:v>2.1772240084642982E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.1676857588961557E-2</c:v>
+                  <c:v>2.2015310890056188E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3092,7 +3097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="609791456"/>
@@ -3154,7 +3159,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fa-IR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="609787192"/>
@@ -3195,7 +3200,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fa-IR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6552,20 +6557,14 @@
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>39420</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>35790</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6582,26 +6581,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>557580</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>81510</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6624,25 +6617,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>328980</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>127230</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6660,25 +6647,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>100380</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>172950</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6700,26 +6681,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>115620</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>73890</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6736,26 +6711,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>130860</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>12930</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7035,16 +7004,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7058,20 +7027,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
       <c r="B2" s="4">
         <f>($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A2))+((A2)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.20589030128179339</v>
+        <v>0.19974070727068258</v>
       </c>
       <c r="D2" s="3">
         <v>5</v>
       </c>
       <c r="E2" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D2))+(D2)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.20747002532011743</v>
+        <v>0.21762362435295637</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>4</v>
@@ -7082,20 +7051,20 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:B31" si="0">($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A3))+((A3)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.10380782222850723</v>
+        <v>0.10073302522295183</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
       </c>
       <c r="E3" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D3))+(D3)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.10451352241667586</v>
+        <v>0.10959032193309533</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -7110,20 +7079,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>7.0163738805238768E-2</v>
+        <v>6.8113874134868496E-2</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E31" si="1">($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D4))+(D4)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>7.0540692451802917E-2</v>
+        <v>7.3925225462749253E-2</v>
       </c>
       <c r="G4" s="2">
         <v>0.81950000000000001</v>
@@ -7138,20 +7107,20 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
-        <v>5.3629254289474716E-2</v>
+        <v>5.2091855786697012E-2</v>
       </c>
       <c r="D5" s="3">
         <v>20</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>5.3813780721572162E-2</v>
+        <v>5.6352180479781896E-2</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -7166,48 +7135,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
-        <v>4.3938609336712432E-2</v>
+        <v>4.2708690534490265E-2</v>
       </c>
       <c r="D6" s="3">
         <v>25</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="1"/>
-        <v>4.3985236285198279E-2</v>
+        <v>4.6015956091766078E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>1.2699999999999999E-2</v>
+        <v>1.231961E-2</v>
       </c>
       <c r="H6" s="2">
         <v>9.5</v>
       </c>
       <c r="J6" s="2">
-        <v>1.2800000000000001E-2</v>
+        <v>1.3428004E-2</v>
       </c>
       <c r="K6" s="2">
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>3.7669884165451029E-2</v>
+        <v>3.6644951830265886E-2</v>
       </c>
       <c r="D7" s="3">
         <v>30</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>3.7605875495752825E-2</v>
+        <v>3.9298142001225986E-2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
@@ -7222,20 +7191,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
-        <v>3.3356541726475848E-2</v>
+        <v>3.2478028296317157E-2</v>
       </c>
       <c r="D8" s="3">
         <v>35</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>3.3197476790266481E-2</v>
+        <v>3.4647990937814906E-2</v>
       </c>
       <c r="G8" s="2">
         <v>8.25E-4</v>
@@ -7250,20 +7219,20 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
-        <v>3.0265313495179549E-2</v>
+        <v>2.9496614243790697E-2</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>3.0020929387254574E-2</v>
+        <v>3.1290129266359441E-2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>10</v>
@@ -7278,20 +7247,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
-        <v>2.7988828069002509E-2</v>
+        <v>2.7305539845545752E-2</v>
       </c>
       <c r="D10" s="3">
         <v>45</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>2.7665616185892292E-2</v>
+        <v>2.8793793856207731E-2</v>
       </c>
       <c r="G10" s="2">
         <v>0.79</v>
@@ -7306,340 +7275,340 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
-        <v>2.6282662606408956E-2</v>
+        <v>2.5667703205297872E-2</v>
       </c>
       <c r="D11" s="3">
         <v>50</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>2.5885166925684749E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.6900526828968648E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
-        <v>2.4991275299148834E-2</v>
+        <v>2.4432221298138764E-2</v>
       </c>
       <c r="D12" s="3">
         <v>55</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>2.4522800531771565E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.544585498930238E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
-        <v>2.4010971608388797E-2</v>
+        <v>2.3498505440796229E-2</v>
       </c>
       <c r="D13" s="3">
         <v>60</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>2.3473996287579148E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.4320129540315726E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
-        <v>2.326996300724421E-2</v>
+        <v>2.2796917314081837E-2</v>
       </c>
       <c r="D14" s="3">
         <v>65</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>2.2666393697018086E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3447439776467238E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>2.2716971976511756E-2</v>
+        <v>2.227771526143241E-2</v>
       </c>
       <c r="D15" s="3">
         <v>70</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>2.2048306691453093E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2773563765227305E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>2.2314395002109008E-2</v>
+        <v>2.1904422068034956E-2</v>
       </c>
       <c r="D16" s="3">
         <v>75</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>2.1581832153884956E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2258738756074221E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>2.203402944847415E-2</v>
+        <v>2.1649679822779728E-2</v>
       </c>
       <c r="D17" s="3">
         <v>80</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>2.1238542746564264E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1873142686116696E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>2.1854308594295206E-2</v>
+        <v>2.1492567770112218E-2</v>
       </c>
       <c r="D18" s="3">
         <v>85</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>2.0996699917094405E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1593970448437871E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>2.1758458322996183E-2</v>
+        <v>2.1416814211267805E-2</v>
       </c>
       <c r="D19" s="3">
         <v>90</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>2.0839395902500241E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1403484737657963E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>2.1733235910964464E-2</v>
+        <v>2.1409573068274422E-2</v>
       </c>
       <c r="D20" s="3">
         <v>95</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>2.075328246885404E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1287682417950829E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>2.1768047179309954E-2</v>
+        <v>2.1460567478754411E-2</v>
       </c>
       <c r="D21" s="3">
         <v>100</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>2.0727681029013595E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1235360980655545E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="0"/>
-        <v>2.1854315887978759E-2</v>
+        <v>2.1561478077925866E-2</v>
       </c>
       <c r="D22" s="3">
         <v>105</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
-        <v>2.0753947012435235E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1237451728284708E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" si="0"/>
-        <v>2.1985025113290438E-2</v>
+        <v>2.1705498112785406E-2</v>
       </c>
       <c r="D23" s="3">
         <v>110</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>2.0825007588674123E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1286534817439532E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="0"/>
-        <v>2.2154378266117655E-2</v>
+        <v>2.1887004613460666E-2</v>
       </c>
       <c r="D24" s="3">
         <v>115</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="1"/>
-        <v>2.0935019984754107E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1376480812268846E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="0"/>
-        <v>2.235754485552097E-2</v>
+        <v>2.2101311771724683E-2</v>
       </c>
       <c r="D25" s="3">
         <v>120</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
-        <v>2.1079115223195038E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1502181849563328E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="0"/>
-        <v>2.2590467269111247E-2</v>
+        <v>2.2344483508666815E-2</v>
       </c>
       <c r="D26" s="3">
         <v>125</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="1"/>
-        <v>2.1253203362913611E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1659347324227165E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="0"/>
-        <v>2.2849712142559223E-2</v>
+        <v>2.2613189295978036E-2</v>
       </c>
       <c r="D27" s="3">
         <v>130</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
-        <v>2.145382368453163E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1844346724256204E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="0"/>
-        <v>2.3132354758102928E-2</v>
+        <v>2.2904592016950678E-2</v>
       </c>
       <c r="D28" s="3">
         <v>135</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
-        <v>2.1678028167838051E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2054087391276532E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
       <c r="B29" s="4">
         <f t="shared" si="0"/>
-        <v>2.3435888214803545E-2</v>
+        <v>2.3216259857263874E-2</v>
       </c>
       <c r="D29" s="3">
         <v>140</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
-        <v>2.1923289938366255E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2285918475253363E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" si="0"/>
-        <v>2.3758151391162066E-2</v>
+        <v>2.3546096425261693E-2</v>
       </c>
       <c r="D30" s="3">
         <v>145</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>2.2187430656058819E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2537554760639473E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
       <c r="B31" s="4">
         <f t="shared" si="0"/>
-        <v>2.4097271315212717E-2</v>
+        <v>2.3892284848175689E-2</v>
       </c>
       <c r="D31" s="3">
         <v>150</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
-        <v>2.2468562426199309E-2</v>
+        <v>2.280701572729394E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7653,16 +7622,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7676,20 +7645,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
       <c r="B2" s="4">
         <f>($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A2))+((A2)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.20592285492660886</v>
+        <v>0.19977326091549807</v>
       </c>
       <c r="D2" s="3">
         <v>5</v>
       </c>
       <c r="E2" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D2))+(D2)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.20749940304678224</v>
+        <v>0.21765300207962118</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>4</v>
@@ -7700,20 +7669,20 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:B31" si="0">($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A3))+((A3)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.10387292951813822</v>
+        <v>0.10079813251258282</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
       </c>
       <c r="E3" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D3))+(D3)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.10457227787000545</v>
+        <v>0.10964907738642492</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -7728,20 +7697,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>7.0261399739685246E-2</v>
+        <v>6.8211535069314974E-2</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E31" si="1">($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D4))+(D4)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>7.0628825631797315E-2</v>
+        <v>7.4013358642743637E-2</v>
       </c>
       <c r="G4" s="2">
         <v>0.81950000000000001</v>
@@ -7756,20 +7725,20 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
-        <v>5.3759468868736678E-2</v>
+        <v>5.2222070365958981E-2</v>
       </c>
       <c r="D5" s="3">
         <v>20</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>5.3931291628231362E-2</v>
+        <v>5.6469691386441097E-2</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -7784,48 +7753,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
-        <v>4.4101377560789898E-2</v>
+        <v>4.2871458758567731E-2</v>
       </c>
       <c r="D6" s="3">
         <v>25</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="1"/>
-        <v>4.4132124918522267E-2</v>
+        <v>4.6162844725090066E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>1.2699999999999999E-2</v>
+        <v>1.231961E-2</v>
       </c>
       <c r="H6" s="2">
         <v>9.5</v>
       </c>
       <c r="J6" s="2">
-        <v>1.2800000000000001E-2</v>
+        <v>1.3428004E-2</v>
       </c>
       <c r="K6" s="2">
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>3.7865206034343978E-2</v>
+        <v>3.6840273699158842E-2</v>
       </c>
       <c r="D7" s="3">
         <v>30</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>3.7782141855741608E-2</v>
+        <v>3.9474408361214776E-2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
@@ -7840,20 +7809,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
-        <v>3.3584417240184287E-2</v>
+        <v>3.2705903810025604E-2</v>
       </c>
       <c r="D8" s="3">
         <v>35</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>3.3403120876920059E-2</v>
+        <v>3.4853635024468484E-2</v>
       </c>
       <c r="G8" s="2">
         <v>8.25E-4</v>
@@ -7868,20 +7837,20 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
-        <v>3.0525742653703485E-2</v>
+        <v>2.9757043402314633E-2</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>3.0255951200572947E-2</v>
+        <v>3.1525151079677814E-2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>10</v>
@@ -7896,20 +7865,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
-        <v>2.8281810872341943E-2</v>
+        <v>2.7598522648885185E-2</v>
       </c>
       <c r="D10" s="3">
         <v>45</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>2.7930015725875463E-2</v>
+        <v>2.9058193396190906E-2</v>
       </c>
       <c r="G10" s="2">
         <v>0.79</v>
@@ -7924,340 +7893,340 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
-        <v>2.660819905456388E-2</v>
+        <v>2.5993239653452797E-2</v>
       </c>
       <c r="D11" s="3">
         <v>50</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>2.6178944192332722E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.7194304095616621E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
-        <v>2.5349365392119252E-2</v>
+        <v>2.4790311391109179E-2</v>
       </c>
       <c r="D12" s="3">
         <v>55</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>2.4845955525084333E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.5769009982615151E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
-        <v>2.4401615346174708E-2</v>
+        <v>2.3889149178582141E-2</v>
       </c>
       <c r="D13" s="3">
         <v>60</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>2.3826529007556711E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.4672662260293292E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
-        <v>2.3693160389845608E-2</v>
+        <v>2.3220114696683242E-2</v>
       </c>
       <c r="D14" s="3">
         <v>65</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>2.3048304143660447E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3829350223109599E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>2.3172723003928648E-2</v>
+        <v>2.2733466288849306E-2</v>
       </c>
       <c r="D15" s="3">
         <v>70</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>2.2459594864760252E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3184851938534465E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>2.2802699674341394E-2</v>
+        <v>2.2392726740267339E-2</v>
       </c>
       <c r="D16" s="3">
         <v>75</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>2.202249805385691E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2699404656046175E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>2.255488776552203E-2</v>
+        <v>2.2170538139827604E-2</v>
       </c>
       <c r="D17" s="3">
         <v>80</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>2.1708586373201017E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2343186312753449E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>2.2407720556158577E-2</v>
+        <v>2.2045979731975588E-2</v>
       </c>
       <c r="D18" s="3">
         <v>85</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>2.1496121270395956E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2093391801739422E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>2.2344423929675044E-2</v>
+        <v>2.2002779817946669E-2</v>
       </c>
       <c r="D19" s="3">
         <v>90</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>2.1368194982466591E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1932283817624312E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>2.2351755162458822E-2</v>
+        <v>2.2028092319768777E-2</v>
       </c>
       <c r="D20" s="3">
         <v>95</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>2.1311459275485185E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.184585922458197E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>2.2419120075619799E-2</v>
+        <v>2.2111640375064259E-2</v>
       </c>
       <c r="D21" s="3">
         <v>100</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>2.1315235562309534E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1822915513951484E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="0"/>
-        <v>2.2537942429104101E-2</v>
+        <v>2.2245104619051208E-2</v>
       </c>
       <c r="D22" s="3">
         <v>105</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
-        <v>2.1370879272395969E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1854383988245449E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" si="0"/>
-        <v>2.270120529923127E-2</v>
+        <v>2.2421678298726239E-2</v>
       </c>
       <c r="D23" s="3">
         <v>110</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>2.1471317575299662E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1932844804065068E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="0"/>
-        <v>2.2903112096873981E-2</v>
+        <v>2.2635738444216989E-2</v>
       </c>
       <c r="D24" s="3">
         <v>115</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="1"/>
-        <v>2.1610707698044438E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2052168525559173E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="0"/>
-        <v>2.3138832331092787E-2</v>
+        <v>2.2882599247296503E-2</v>
       </c>
       <c r="D25" s="3">
         <v>120</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
-        <v>2.1784180663150167E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2207247289518457E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="0"/>
-        <v>2.3404308389498554E-2</v>
+        <v>2.3158324629054126E-2</v>
       </c>
       <c r="D26" s="3">
         <v>125</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="1"/>
-        <v>2.1987646529533538E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2393790490847092E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="0"/>
-        <v>2.3696106907762023E-2</v>
+        <v>2.3459584061180837E-2</v>
       </c>
       <c r="D27" s="3">
         <v>130</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
-        <v>2.2217644577816352E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.260816761754093E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="0"/>
-        <v>2.4011303168121223E-2</v>
+        <v>2.3783540426968973E-2</v>
       </c>
       <c r="D28" s="3">
         <v>135</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
-        <v>2.2471226787787572E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2847286011226053E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
       <c r="B29" s="4">
         <f t="shared" si="0"/>
-        <v>2.434739026963733E-2</v>
+        <v>2.4127761912097659E-2</v>
       </c>
       <c r="D29" s="3">
         <v>140</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
-        <v>2.2745866284980574E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3108494821867675E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" si="0"/>
-        <v>2.4702207090811348E-2</v>
+        <v>2.4490152124910975E-2</v>
       </c>
       <c r="D30" s="3">
         <v>145</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>2.3039384729337933E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.338950883391859E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
       <c r="B31" s="4">
         <f t="shared" si="0"/>
-        <v>2.5073880659677493E-2</v>
+        <v>2.4868894192640465E-2</v>
       </c>
       <c r="D31" s="3">
         <v>150</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
-        <v>2.3349894226143222E-2</v>
+        <v>2.3688347527237853E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8271,16 +8240,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8294,20 +8263,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>5</v>
       </c>
       <c r="B2" s="4">
         <f>($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A2))+((A2)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.20586105817712863</v>
+        <v>0.19971146416601782</v>
       </c>
       <c r="D2" s="3">
         <v>5</v>
       </c>
       <c r="E2" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D2))+(D2)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.20744363515887621</v>
+        <v>0.21759723419171514</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>4</v>
@@ -8318,20 +8287,20 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>10</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:B31" si="0">($G$6*(0.5*$G$8*($G$10*$H$10)^2)*($G$4/(A3))+((A3)/((0.5*$G$8*($G$10*$H$10)^2)*3.14*$H$6*$H$8*$G$4)))*$H$4</f>
-        <v>0.1037493360191777</v>
+        <v>0.10067453901362231</v>
       </c>
       <c r="D3" s="3">
         <v>10</v>
       </c>
       <c r="E3" s="4">
         <f>($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D3))+(D3)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>0.10446074209419333</v>
+        <v>0.1095375416106128</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -8346,20 +8315,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>15</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>7.0076009491244484E-2</v>
+        <v>6.8026144820874213E-2</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E31" si="1">($J$6*(0.5*$J$8*($J$10*$K$10)^2)*($J$4/(D4))+(D4)/(((0.5*$J$8*($J$10*$K$10)^2)*3.14*$K$6*$K$8)*$J$4))*$K$4</f>
-        <v>7.0461521968079144E-2</v>
+        <v>7.384605497902548E-2</v>
       </c>
       <c r="G4" s="2">
         <v>0.81950000000000001</v>
@@ -8374,20 +8343,20 @@
         <v>0.37440000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
-        <v>5.3512281870815658E-2</v>
+        <v>5.1974883368037961E-2</v>
       </c>
       <c r="D5" s="3">
         <v>20</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>5.3708220076607131E-2</v>
+        <v>5.6246619834816873E-2</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>6</v>
@@ -8402,48 +8371,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>25</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
-        <v>4.3792393813388612E-2</v>
+        <v>4.2562475011166452E-2</v>
       </c>
       <c r="D6" s="3">
         <v>25</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="1"/>
-        <v>4.3853285478991991E-2</v>
+        <v>4.588400528555979E-2</v>
       </c>
       <c r="G6" s="2">
-        <v>1.2699999999999999E-2</v>
+        <v>1.231961E-2</v>
       </c>
       <c r="H6" s="2">
         <v>9.5</v>
       </c>
       <c r="J6" s="2">
-        <v>1.2800000000000001E-2</v>
+        <v>1.3428004E-2</v>
       </c>
       <c r="K6" s="2">
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>30</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>3.7494425537462441E-2</v>
+        <v>3.6469493202277305E-2</v>
       </c>
       <c r="D7" s="3">
         <v>30</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>3.7447534528305272E-2</v>
+        <v>3.913980103377844E-2</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
@@ -8458,20 +8427,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>35</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
-        <v>3.3151839993822492E-2</v>
+        <v>3.2273326563663808E-2</v>
       </c>
       <c r="D8" s="3">
         <v>35</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>3.3012745661577671E-2</v>
+        <v>3.4463259809126096E-2</v>
       </c>
       <c r="G8" s="2">
         <v>8.25E-4</v>
@@ -8486,20 +8455,20 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>40</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
-        <v>3.0031368657861435E-2</v>
+        <v>2.9262669406472583E-2</v>
       </c>
       <c r="D9" s="3">
         <v>40</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>2.9809808097324503E-2</v>
+        <v>3.107900797642937E-2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>10</v>
@@ -8514,20 +8483,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
-        <v>2.772564012701963E-2</v>
+        <v>2.7042351903562876E-2</v>
       </c>
       <c r="D10" s="3">
         <v>45</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>2.7428104734720966E-2</v>
+        <v>2.8556282405036409E-2</v>
       </c>
       <c r="G10" s="2">
         <v>0.79</v>
@@ -8542,340 +8511,340 @@
         <v>986</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>50</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
-        <v>2.5990231559761313E-2</v>
+        <v>2.5375272158650229E-2</v>
       </c>
       <c r="D11" s="3">
         <v>50</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>2.5621265313272166E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.6636625216556065E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>55</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
-        <v>2.4669601147836426E-2</v>
+        <v>2.4110547146826353E-2</v>
       </c>
       <c r="D12" s="3">
         <v>55</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>2.4232508758117725E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.515556321564854E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>60</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
-        <v>2.3660054352411627E-2</v>
+        <v>2.314758818481906E-2</v>
       </c>
       <c r="D13" s="3">
         <v>60</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>2.3157314352684043E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.4003447605420627E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>65</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
-        <v>2.2889802646602272E-2</v>
+        <v>2.2416756953439903E-2</v>
       </c>
       <c r="D14" s="3">
         <v>65</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>2.2323321600881726E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.3104367680330879E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>70</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>2.2307568511205054E-2</v>
+        <v>2.1868311796125712E-2</v>
       </c>
       <c r="D15" s="3">
         <v>70</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>2.1678844434075476E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.2404101507849689E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>75</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>2.1875748432137545E-2</v>
+        <v>2.1465775498063493E-2</v>
       </c>
       <c r="D16" s="3">
         <v>75</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>2.1185979735266078E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1862886337455343E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>80</v>
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>2.1566139773837922E-2</v>
+        <v>2.11817901481435E-2</v>
       </c>
       <c r="D17" s="3">
         <v>80</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>2.0816300166704129E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1450900106256564E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>85</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>2.1357175814994214E-2</v>
+        <v>2.0995434990811222E-2</v>
       </c>
       <c r="D18" s="3">
         <v>85</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>2.0548067175993015E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1145337707336478E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>90</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>2.1232082439030426E-2</v>
+        <v>2.0890438327302047E-2</v>
       </c>
       <c r="D19" s="3">
         <v>90</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>2.0364373000157594E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0928461835315316E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>95</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>2.1177616922333942E-2</v>
+        <v>2.08539540796439E-2</v>
       </c>
       <c r="D20" s="3">
         <v>95</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>2.0251869405270129E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0786269354366917E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>100</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>2.1183185086014664E-2</v>
+        <v>2.0875705385459124E-2</v>
       </c>
       <c r="D21" s="3">
         <v>100</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>2.0199877804188429E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0707557755830379E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>105</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="0"/>
-        <v>2.1240210690018708E-2</v>
+        <v>2.0947372879965814E-2</v>
       </c>
       <c r="D22" s="3">
         <v>105</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="1"/>
-        <v>2.0199753626368808E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0683258342218284E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>110</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" si="0"/>
-        <v>2.1341676810665625E-2</v>
+        <v>2.1062149810160587E-2</v>
       </c>
       <c r="D23" s="3">
         <v>110</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="1"/>
-        <v>2.0244424041366442E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0705951270131851E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="0"/>
-        <v>2.1481786858828077E-2</v>
+        <v>2.1214413206171085E-2</v>
       </c>
       <c r="D24" s="3">
         <v>115</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="1"/>
-        <v>2.0328046276205162E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.07695071037199E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>120</v>
       </c>
       <c r="B25" s="4">
         <f t="shared" si="0"/>
-        <v>2.1655710343566628E-2</v>
+        <v>2.1399477259770341E-2</v>
       </c>
       <c r="D25" s="3">
         <v>120</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="1"/>
-        <v>2.0445751353404835E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0868817979773125E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>125</v>
       </c>
       <c r="B26" s="4">
         <f t="shared" si="0"/>
-        <v>2.185938965249214E-2</v>
+        <v>2.1613405892047705E-2</v>
       </c>
       <c r="D26" s="3">
         <v>125</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="1"/>
-        <v>2.0593449331882147E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.0999593293195708E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>130</v>
       </c>
       <c r="B27" s="4">
         <f t="shared" si="0"/>
-        <v>2.2089391421275351E-2</v>
+        <v>2.1852868574694165E-2</v>
       </c>
       <c r="D27" s="3">
         <v>130</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
-        <v>2.0767679492258911E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1158202531983489E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>135</v>
       </c>
       <c r="B28" s="4">
         <f t="shared" si="0"/>
-        <v>2.2342790932154293E-2</v>
+        <v>2.2115028191002042E-2</v>
       </c>
       <c r="D28" s="3">
         <v>135</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
-        <v>2.0965493814324072E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1341553037762556E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>140</v>
       </c>
       <c r="B29" s="4">
         <f t="shared" si="0"/>
-        <v>2.2617081284190141E-2</v>
+        <v>2.239745292665047E-2</v>
       </c>
       <c r="D29" s="3">
         <v>140</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
-        <v>2.1184365423611021E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1546993960498126E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>145</v>
       </c>
       <c r="B30" s="4">
         <f t="shared" si="0"/>
-        <v>2.2910101355883904E-2</v>
+        <v>2.2698046389983535E-2</v>
       </c>
       <c r="D30" s="3">
         <v>145</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>2.1422115980062328E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2.1772240084642982E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>150</v>
       </c>
       <c r="B31" s="4">
         <f t="shared" si="0"/>
-        <v>2.3219978175269787E-2</v>
+        <v>2.3014991708232759E-2</v>
       </c>
       <c r="D31" s="3">
         <v>150</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
-        <v>2.1676857588961557E-2</v>
+        <v>2.2015310890056188E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>